<commit_message>
can search for manual landmarks
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_evaluation/landmark_points.xlsx
+++ b/franz_hsa/landmark_evaluation/landmark_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9C899-B122-4F20-9749-4BEB5A8BE7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5464A1-2234-47E5-AD7D-0281474AB55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -494,7 +494,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -518,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -526,7 +526,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -534,7 +534,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -542,7 +542,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -558,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -566,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -574,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -582,7 +582,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -590,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -598,7 +598,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -606,7 +606,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -614,7 +614,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -622,7 +622,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -630,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -638,7 +638,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,7 +646,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -654,7 +654,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -670,7 +670,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -678,7 +678,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -686,7 +686,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
annotating 27 landmark points
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_evaluation/landmark_points.xlsx
+++ b/franz_hsa/landmark_evaluation/landmark_points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5464A1-2234-47E5-AD7D-0281474AB55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D27EA9-0B1C-4BBC-8F5B-C0F09F1275EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +478,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -486,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -494,127 +494,103 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>3</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>9</v>
+        <v>9395</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>12</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
-        <v>13</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
-        <v>14</v>
-      </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
-        <v>15</v>
-      </c>
+      <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
-        <v>16</v>
-      </c>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1">
-        <v>17</v>
-      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>18</v>
+        <v>8948</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -622,7 +598,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>19</v>
+        <v>678</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -630,7 +606,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>20</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -638,7 +614,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>21</v>
+        <v>4197</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -646,48 +622,40 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>22</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1">
-        <v>23</v>
-      </c>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
-        <v>24</v>
-      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>25</v>
+        <v>8967</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="1">
-        <v>26</v>
-      </c>
+      <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1">
-        <v>27</v>
-      </c>
+      <c r="B28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
annotated the 27 landmarks
</commit_message>
<xml_diff>
--- a/franz_hsa/landmark_evaluation/landmark_points.xlsx
+++ b/franz_hsa/landmark_evaluation/landmark_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\work\projects\arp\quantification-methods\hsa\3dphoto\franz_hsa\landmark_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D27EA9-0B1C-4BBC-8F5B-C0F09F1275EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA939B5-732B-4BE6-A0A1-D8DAE9E4E859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11196" yWindow="12912" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,15 +457,15 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -473,7 +473,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>4869</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -489,7 +489,7 @@
         <v>3410</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -497,103 +497,127 @@
         <v>2431</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>5752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>7395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>8614</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>9395</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>4328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>8232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>3607</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>5549</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>10595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>6576</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>8948</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -601,7 +625,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -609,7 +633,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -617,7 +641,7 @@
         <v>4197</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -625,37 +649,45 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>8967</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>9124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1">
+        <v>6083</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>